<commit_message>
completed pca analysis and plots
</commit_message>
<xml_diff>
--- a/Data/params_struc.xlsx
+++ b/Data/params_struc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pramodhegde/Documents/DSA/chapter_1/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2E7415-2A04-6A4F-BC31-378EF111C1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CE4A26-8B6A-924A-BE24-E8DB1358F15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60826,8 +60826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AN2" sqref="AN2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>